<commit_message>
Add new cable CBL14_24V_open
</commit_message>
<xml_diff>
--- a/Docs/AT-ETX-2i10G.CBL14_24V.xlsx
+++ b/Docs/AT-ETX-2i10G.CBL14_24V.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2i-10G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8105260D-7CE4-493E-8BEE-CD6BDF431B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDBA4B-F5BD-4B13-98DB-48876C8F1E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="1230" windowWidth="21600" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="2745" windowWidth="17025" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -896,11 +896,11 @@
         <v>15</v>
       </c>
       <c r="C22" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ref="D22" si="0">$C$16*C22</f>
-        <v>800</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>